<commit_message>
fixed value in zombies table
</commit_message>
<xml_diff>
--- a/HelpfulMaterials/zombies information.xlsx
+++ b/HelpfulMaterials/zombies information.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Documents\GitHub\codegurubyteme\HelpfulMaterials\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D8C6721B-7FB5-459A-A61A-779CAF955048}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6DD02FF-4ACB-4157-A7A2-2FA2DF78D601}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C309F57C-6882-4361-8EB0-F1827C16452A}"/>
+    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="8964" xr2:uid="{C309F57C-6882-4361-8EB0-F1827C16452A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -114,9 +114,6 @@
     <t>0x8346</t>
   </si>
   <si>
-    <t>0x3FAA</t>
-  </si>
-  <si>
     <t>0xEB3F</t>
   </si>
   <si>
@@ -124,6 +121,9 @@
   </si>
   <si>
     <t>0x100 * Y</t>
+  </si>
+  <si>
+    <t>0x3FE6</t>
   </si>
 </sst>
 </file>
@@ -491,8 +491,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE841EB0-3A24-4396-9D3E-0BE85B044EA2}">
   <dimension ref="F6:I14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" topLeftCell="B4" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -554,7 +554,7 @@
         <v>16</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>13</v>
@@ -596,7 +596,7 @@
         <v>19</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="I12" s="1" t="s">
         <v>12</v>
@@ -610,7 +610,7 @@
         <v>20</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I13" s="1" t="s">
         <v>12</v>
@@ -624,7 +624,7 @@
         <v>21</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I14" s="1" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
added a lot of smart variations
</commit_message>
<xml_diff>
--- a/HelpfulMaterials/zombies information.xlsx
+++ b/HelpfulMaterials/zombies information.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Documents\GitHub\codegurubyteme\HelpfulMaterials\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6DD02FF-4ACB-4157-A7A2-2FA2DF78D601}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B6FC8F0-4C47-462B-A8A7-0EFC7A3E9509}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="8964" xr2:uid="{C309F57C-6882-4361-8EB0-F1827C16452A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C309F57C-6882-4361-8EB0-F1827C16452A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="40">
   <si>
     <t>dist from start</t>
   </si>
@@ -124,6 +124,36 @@
   </si>
   <si>
     <t>0x3FE6</t>
+  </si>
+  <si>
+    <t>word / byte</t>
+  </si>
+  <si>
+    <t>word</t>
+  </si>
+  <si>
+    <t>0x46</t>
+  </si>
+  <si>
+    <t>byte</t>
+  </si>
+  <si>
+    <t>0xFFE2</t>
+  </si>
+  <si>
+    <t>0x0000</t>
+  </si>
+  <si>
+    <t>0xFFE6</t>
+  </si>
+  <si>
+    <t>0x3F</t>
+  </si>
+  <si>
+    <t>0xFFCC</t>
+  </si>
+  <si>
+    <t>0xFFB9</t>
   </si>
 </sst>
 </file>
@@ -489,10 +519,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE841EB0-3A24-4396-9D3E-0BE85B044EA2}">
-  <dimension ref="F6:I14"/>
+  <dimension ref="F6:J22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" topLeftCell="B7" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -502,9 +532,10 @@
     <col min="7" max="7" width="13.6640625" customWidth="1"/>
     <col min="8" max="8" width="15.6640625" customWidth="1"/>
     <col min="9" max="9" width="11.6640625" customWidth="1"/>
+    <col min="10" max="10" width="11.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="6:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="6:10" x14ac:dyDescent="0.3">
       <c r="F6" s="2" t="s">
         <v>1</v>
       </c>
@@ -515,10 +546,13 @@
         <v>2</v>
       </c>
       <c r="I6" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="J6" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="6:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="6:10" x14ac:dyDescent="0.3">
       <c r="F7" s="1" t="s">
         <v>4</v>
       </c>
@@ -529,10 +563,13 @@
         <v>22</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="6:9" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="6:10" x14ac:dyDescent="0.3">
       <c r="F8" s="1" t="s">
         <v>5</v>
       </c>
@@ -543,10 +580,13 @@
         <v>23</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="6:9" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="6:10" x14ac:dyDescent="0.3">
       <c r="F9" s="1" t="s">
         <v>6</v>
       </c>
@@ -557,10 +597,13 @@
         <v>28</v>
       </c>
       <c r="I9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J9" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="6:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="6:10" x14ac:dyDescent="0.3">
       <c r="F10" s="1" t="s">
         <v>7</v>
       </c>
@@ -571,10 +614,13 @@
         <v>24</v>
       </c>
       <c r="I10" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J10" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="6:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="6:10" x14ac:dyDescent="0.3">
       <c r="F11" s="1" t="s">
         <v>8</v>
       </c>
@@ -585,10 +631,13 @@
         <v>25</v>
       </c>
       <c r="I11" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J11" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="6:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="6:10" x14ac:dyDescent="0.3">
       <c r="F12" s="1" t="s">
         <v>9</v>
       </c>
@@ -599,10 +648,13 @@
         <v>29</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="6:9" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="6:10" x14ac:dyDescent="0.3">
       <c r="F13" s="1" t="s">
         <v>10</v>
       </c>
@@ -613,10 +665,13 @@
         <v>26</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="6:9" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="6:10" x14ac:dyDescent="0.3">
       <c r="F14" s="1" t="s">
         <v>11</v>
       </c>
@@ -627,6 +682,145 @@
         <v>27</v>
       </c>
       <c r="I14" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="6:10" x14ac:dyDescent="0.3">
+      <c r="F15" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="6:10" x14ac:dyDescent="0.3">
+      <c r="F16" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="6:10" x14ac:dyDescent="0.3">
+      <c r="F17" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="6:10" x14ac:dyDescent="0.3">
+      <c r="F18" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="6:10" x14ac:dyDescent="0.3">
+      <c r="F19" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="6:10" x14ac:dyDescent="0.3">
+      <c r="F20" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="6:10" x14ac:dyDescent="0.3">
+      <c r="F21" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="6:10" x14ac:dyDescent="0.3">
+      <c r="F22" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="J22" s="1" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>